<commit_message>
updated daq circuit board pinout and cleaned up .gitignore files
</commit_message>
<xml_diff>
--- a/lab/daq_circuit_board_pinout.xlsx
+++ b/lab/daq_circuit_board_pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonic\Documents\DREXEL UNIVERSITY\t8_f\ECE 303\ece303\lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9D1F7D09-616E-4FEA-A89A-B4546E45FA2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65B6F30A-CE93-4F08-A97B-3D2712050D02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9540" xr2:uid="{6CE14227-086A-4F38-B90D-EC596DD10CE8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>A</t>
   </si>
@@ -165,9 +165,6 @@
     <t>7 SEGMENT - C</t>
   </si>
   <si>
-    <t>7 SEGMENT - DATA</t>
-  </si>
-  <si>
     <t>7 SEGMENT - E</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>+3.3V</t>
+  </si>
+  <si>
+    <t>7 SEGMENT - D</t>
   </si>
 </sst>
 </file>
@@ -263,12 +263,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -586,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53AC1-70BB-4A95-AE74-2627E9797BDE}">
-  <dimension ref="A2:H28"/>
+  <dimension ref="A2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -597,7 +596,7 @@
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="23.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.125" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -609,7 +608,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -633,7 +638,7 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H4" t="s">
@@ -647,7 +652,7 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H5" t="s">
@@ -675,7 +680,7 @@
       <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H7" t="s">
@@ -689,7 +694,7 @@
       <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H8" t="s">
@@ -709,6 +714,9 @@
       <c r="D9" t="s">
         <v>42</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -717,11 +725,14 @@
       <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" t="s">
-        <v>43</v>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -732,10 +743,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -745,11 +759,14 @@
       <c r="B12" s="1">
         <v>11</v>
       </c>
-      <c r="G12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -760,10 +777,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -773,11 +793,14 @@
       <c r="B14" s="1">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" t="s">
-        <v>45</v>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -787,11 +810,14 @@
       <c r="B15" s="1">
         <v>14</v>
       </c>
-      <c r="G15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" t="s">
-        <v>46</v>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -802,41 +828,50 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
-      <c r="G17" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
+      <c r="C18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H18" t="s">
+      <c r="D18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -844,77 +879,101 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
       </c>
-      <c r="G20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
       </c>
-      <c r="G21" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
       </c>
-      <c r="G22" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -931,28 +990,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
-        <v>64</v>
-      </c>
-      <c r="H27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrating 7 segment and accelerometer
</commit_message>
<xml_diff>
--- a/lab/daq_circuit_board_pinout.xlsx
+++ b/lab/daq_circuit_board_pinout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonic\Documents\DREXEL UNIVERSITY\t8_f\ECE 303\ece303\lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonic\Documents\DREXEL UNIVERSITY\t8_f\ECE_303\ece303\lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65B6F30A-CE93-4F08-A97B-3D2712050D02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8BA02466-CEAF-4957-842E-3CA9750C2BB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9540" xr2:uid="{6CE14227-086A-4F38-B90D-EC596DD10CE8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" xr2:uid="{6CE14227-086A-4F38-B90D-EC596DD10CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
   <si>
     <t>A</t>
   </si>
@@ -229,6 +229,48 @@
   </si>
   <si>
     <t>7 SEGMENT - D</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>BLU</t>
+  </si>
+  <si>
+    <t>Start stop</t>
+  </si>
+  <si>
+    <t>H-Bridge</t>
+  </si>
+  <si>
+    <t>+12V</t>
+  </si>
+  <si>
+    <t>PWM Signal</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Relay Pin</t>
+  </si>
+  <si>
+    <t>D_OUT_49</t>
+  </si>
+  <si>
+    <t>D_OUT_12</t>
   </si>
 </sst>
 </file>
@@ -585,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53AC1-70BB-4A95-AE74-2627E9797BDE}">
-  <dimension ref="A2:H31"/>
+  <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -596,6 +638,7 @@
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="23.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.125" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.25" customWidth="1"/>
   </cols>
@@ -1005,6 +1048,141 @@
         <v>36</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>13</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>14</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
working payload from DAQ to main_controller
</commit_message>
<xml_diff>
--- a/lab/daq_circuit_board_pinout.xlsx
+++ b/lab/daq_circuit_board_pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonic\Documents\DREXEL UNIVERSITY\t8_f\ECE_303\ece303\lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E0AB4D74-2844-4651-9604-F41687C25339}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{398DFC56-E75A-4461-800B-616772C9B1BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" xr2:uid="{6CE14227-086A-4F38-B90D-EC596DD10CE8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7560" xr2:uid="{6CE14227-086A-4F38-B90D-EC596DD10CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>D_OUT_32</t>
   </si>
   <si>
-    <t>A_IN_X</t>
-  </si>
-  <si>
     <t>BATTERY</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>D_IN_2</t>
+  </si>
+  <si>
+    <t>A_IN_4</t>
   </si>
 </sst>
 </file>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53AC1-70BB-4A95-AE74-2627E9797BDE}">
   <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -687,10 +687,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
         <v>64</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>37</v>
@@ -978,7 +978,7 @@
         <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>37</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1086,13 +1086,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
         <v>76</v>
-      </c>
-      <c r="F37" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1110,13 +1110,13 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1124,13 +1124,13 @@
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
         <v>90</v>
       </c>
-      <c r="D41" t="s">
-        <v>91</v>
-      </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
         <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1149,13 +1149,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
         <v>87</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1163,13 +1163,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1177,13 +1177,13 @@
         <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s">
         <v>82</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>83</v>
-      </c>
-      <c r="E45" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1191,10 +1191,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E46" t="s">
         <v>34</v>
@@ -1205,13 +1205,13 @@
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1219,13 +1219,13 @@
         <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" t="s">
         <v>74</v>
       </c>
-      <c r="D48" t="s">
-        <v>75</v>
-      </c>
       <c r="E48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,13 +1233,13 @@
         <v>12</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1247,13 +1247,13 @@
         <v>13</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1264,10 +1264,10 @@
         <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>